<commit_message>
1. updated tax columns for detailed correctness
</commit_message>
<xml_diff>
--- a/phinCalc.xlsx
+++ b/phinCalc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/junle/Dropbox/ProjectJZ/finCalc/phinCalc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB08C8BC-29B8-BE44-A755-A749B99F9C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5381FA26-0D0F-634F-AE1D-8608BC013988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,15 +64,6 @@
     <t>rate (%)</t>
   </si>
   <si>
-    <t>from</t>
-  </si>
-  <si>
-    <t>up to</t>
-  </si>
-  <si>
-    <t>and up</t>
-  </si>
-  <si>
     <t>state tax rates</t>
   </si>
   <si>
@@ -116,6 +107,15 @@
   </si>
   <si>
     <t>end of 30-year mortgage</t>
+  </si>
+  <si>
+    <t>over</t>
+  </si>
+  <si>
+    <t>but not over</t>
+  </si>
+  <si>
+    <t>and over</t>
   </si>
 </sst>
 </file>
@@ -1683,10 +1683,10 @@
         <v>7</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="K14" s="10"/>
     </row>
@@ -1706,8 +1706,8 @@
         <v>12</v>
       </c>
       <c r="D16" s="5">
-        <f>E15+1</f>
-        <v>11001</v>
+        <f>E15</f>
+        <v>11000</v>
       </c>
       <c r="E16" s="12">
         <v>44725</v>
@@ -1718,8 +1718,8 @@
         <v>22</v>
       </c>
       <c r="D17" s="5">
-        <f t="shared" ref="D17:D21" si="0">E16+1</f>
-        <v>44726</v>
+        <f t="shared" ref="D17:D21" si="0">E16</f>
+        <v>44725</v>
       </c>
       <c r="E17" s="12">
         <v>95375</v>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="D18" s="5">
         <f t="shared" si="0"/>
-        <v>95376</v>
+        <v>95375</v>
       </c>
       <c r="E18" s="12">
         <v>182100</v>
@@ -1743,7 +1743,7 @@
       </c>
       <c r="D19" s="5">
         <f t="shared" si="0"/>
-        <v>182101</v>
+        <v>182100</v>
       </c>
       <c r="E19" s="12">
         <v>231250</v>
@@ -1755,7 +1755,7 @@
       </c>
       <c r="D20" s="5">
         <f t="shared" si="0"/>
-        <v>231251</v>
+        <v>231250</v>
       </c>
       <c r="E20" s="12">
         <v>578125</v>
@@ -1767,15 +1767,15 @@
       </c>
       <c r="D21" s="5">
         <f t="shared" si="0"/>
-        <v>578126</v>
+        <v>578125</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C24" s="25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="23"/>
@@ -1785,10 +1785,10 @@
         <v>7</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.2">
@@ -1807,8 +1807,8 @@
         <v>2</v>
       </c>
       <c r="D27" s="5">
-        <f>E26+1</f>
-        <v>10413</v>
+        <f>E26</f>
+        <v>10412</v>
       </c>
       <c r="E27" s="12">
         <v>24684</v>
@@ -1819,8 +1819,8 @@
         <v>4</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" ref="D28:D34" si="1">E27+1</f>
-        <v>24685</v>
+        <f t="shared" ref="D28:D34" si="1">E27</f>
+        <v>24684</v>
       </c>
       <c r="E28" s="12">
         <v>38959</v>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="D29" s="5">
         <f t="shared" si="1"/>
-        <v>38960</v>
+        <v>38959</v>
       </c>
       <c r="E29" s="12">
         <v>54081</v>
@@ -1844,7 +1844,7 @@
       </c>
       <c r="D30" s="5">
         <f t="shared" si="1"/>
-        <v>54082</v>
+        <v>54081</v>
       </c>
       <c r="E30" s="12">
         <v>68350</v>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="D31" s="5">
         <f t="shared" si="1"/>
-        <v>68351</v>
+        <v>68350</v>
       </c>
       <c r="E31" s="12">
         <v>349137</v>
@@ -1868,7 +1868,7 @@
       </c>
       <c r="D32" s="5">
         <f t="shared" si="1"/>
-        <v>349138</v>
+        <v>349137</v>
       </c>
       <c r="E32" s="12">
         <v>418961</v>
@@ -1880,7 +1880,7 @@
       </c>
       <c r="D33" s="5">
         <f t="shared" si="1"/>
-        <v>418962</v>
+        <v>418961</v>
       </c>
       <c r="E33" s="12">
         <v>698271</v>
@@ -1892,10 +1892,10 @@
       </c>
       <c r="D34" s="5">
         <f t="shared" si="1"/>
-        <v>698272</v>
+        <v>698271</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.2">
@@ -1903,11 +1903,11 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="D37" s="26" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="7"/>
@@ -1916,31 +1916,31 @@
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B38" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C38" s="14" t="s">
+      <c r="F38" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="I38" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="J38" s="14" t="s">
         <v>17</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="G38" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H38" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="14" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
@@ -2318,7 +2318,7 @@
         <v>14400</v>
       </c>
       <c r="J54" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.2">
@@ -2497,7 +2497,7 @@
         <v>-568000</v>
       </c>
       <c r="J61" s="16" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="62" spans="2:10" x14ac:dyDescent="0.2">
@@ -2801,7 +2801,7 @@
         <v>-544000</v>
       </c>
       <c r="J73" s="16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
@@ -3120,7 +3120,7 @@
         <v>-336571.42857142858</v>
       </c>
       <c r="J86" s="16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="2:10" x14ac:dyDescent="0.2">
@@ -3247,7 +3247,7 @@
         <v>-90857.14285714287</v>
       </c>
       <c r="J91" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" spans="2:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
1. minor addition to the excel file notes section
</commit_message>
<xml_diff>
--- a/phinCalc.xlsx
+++ b/phinCalc.xlsx
@@ -953,7 +953,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1015,7 +1015,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:t>None</a:t>
+              <a:t/>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1392,15 +1392,16 @@
     <col width="64.83203125" customWidth="1" style="1" min="10" max="10"/>
     <col width="10.83203125" customWidth="1" style="1" min="11" max="11"/>
     <col width="10.83203125" customWidth="1" style="2" min="12" max="12"/>
-    <col width="10.83203125" customWidth="1" style="1" min="13" max="67"/>
-    <col width="10.83203125" customWidth="1" style="1" min="68" max="16384"/>
+    <col width="10.83203125" customWidth="1" style="1" min="13" max="68"/>
+    <col width="10.83203125" customWidth="1" style="1" min="69" max="16384"/>
   </cols>
   <sheetData>
-    <row r="3" ht="112" customFormat="1" customHeight="1" s="8">
+    <row r="3" ht="128" customFormat="1" customHeight="1" s="8">
       <c r="B3" s="23" t="inlineStr">
         <is>
           <t>notes:
 -please fill or check all blue fields
+-then run python script
 -python script outputs are purple fields
 -initial investment amount is assumed to already be taxed
 -if yearly income (after taxes) is greater than yearly expense, the difference will be added to the balance

</xml_diff>